<commit_message>
change of Low bound in Policy
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Policy.xlsx
+++ b/SuppXLS/Scen_SYS_Policy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-DK\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864D261D-4753-469C-A9D2-3D10C2314074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672E7989-F80A-4E78-8016-E949392AC92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14664" yWindow="636" windowWidth="21960" windowHeight="15468" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
@@ -1607,7 +1607,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
@@ -1648,10 +1648,10 @@
   <dimension ref="B4:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="4" spans="2:7">
       <c r="B4" s="10" t="s">
@@ -1747,7 +1747,7 @@
         <v>2400</v>
       </c>
       <c r="F9" s="17">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>24</v>
@@ -1927,9 +1927,9 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -3109,9 +3109,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
@@ -3253,15 +3253,15 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.5546875" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" customWidth="1"/>
-    <col min="24" max="24" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.54296875" customWidth="1"/>
+    <col min="23" max="23" width="13.90625" customWidth="1"/>
+    <col min="24" max="24" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:43">
@@ -3308,7 +3308,7 @@
       <c r="AK3" s="19"/>
       <c r="AL3" s="19"/>
     </row>
-    <row r="4" spans="2:43" ht="18" thickBot="1">
+    <row r="4" spans="2:43" ht="18.5" thickBot="1">
       <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
@@ -3353,7 +3353,7 @@
       <c r="AL4" s="19"/>
       <c r="AM4" s="19"/>
     </row>
-    <row r="5" spans="2:43" ht="43.2">
+    <row r="5" spans="2:43" ht="43.5">
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
@@ -3412,7 +3412,7 @@
       <c r="AL5" s="19"/>
       <c r="AM5" s="19"/>
     </row>
-    <row r="6" spans="2:43" ht="15.6">
+    <row r="6" spans="2:43" ht="15.5">
       <c r="B6" t="s">
         <v>111</v>
       </c>
@@ -3840,7 +3840,7 @@
       <c r="AL12" s="19"/>
       <c r="AM12" s="19"/>
     </row>
-    <row r="13" spans="2:43" ht="28.8">
+    <row r="13" spans="2:43" ht="29">
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="AL15" s="19"/>
       <c r="AM15" s="19"/>
     </row>
-    <row r="16" spans="2:43" ht="43.2">
+    <row r="16" spans="2:43" ht="43.5">
       <c r="O16" s="19"/>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
@@ -4340,7 +4340,7 @@
       <c r="AK23" s="19"/>
       <c r="AL23" s="19"/>
     </row>
-    <row r="24" spans="15:39" ht="27.6">
+    <row r="24" spans="15:39" ht="26">
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="61" t="s">
@@ -5572,7 +5572,7 @@
       <c r="AK57" s="19"/>
       <c r="AL57" s="19"/>
     </row>
-    <row r="58" spans="15:38" ht="15.6">
+    <row r="58" spans="15:38" ht="15.5">
       <c r="O58" s="19"/>
       <c r="P58" s="19"/>
       <c r="Q58" s="19"/>

</xml_diff>

<commit_message>
Policy, remove lower bound DKW2030
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Policy.xlsx
+++ b/SuppXLS/Scen_SYS_Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B8B3A1-8C39-4711-B7C0-955D8A54CF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385A31CB-A8F8-4585-9DE3-16ACD54B3E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1648,7 +1648,7 @@
   <dimension ref="B4:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1764,8 +1764,7 @@
         <v>2030</v>
       </c>
       <c r="E10" s="17">
-        <f>5000-F10</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="F10" s="17">
         <v>0</v>

</xml_diff>

<commit_message>
delete lower bound 2028
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Policy.xlsx
+++ b/SuppXLS/Scen_SYS_Policy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385A31CB-A8F8-4585-9DE3-16ACD54B3E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA666195-E495-44C3-8524-FE71176A0D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1648,7 +1648,7 @@
   <dimension ref="B4:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1744,7 +1744,7 @@
         <v>2028</v>
       </c>
       <c r="E9" s="17">
-        <v>2400</v>
+        <v>0</v>
       </c>
       <c r="F9" s="17">
         <v>0</v>

</xml_diff>